<commit_message>
[NTM:SPACE] Duna temperature rebalance
</commit_message>
<xml_diff>
--- a/DEBUG_SHEET/TEMPS.xlsx
+++ b/DEBUG_SHEET/TEMPS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0BF18CF-6267-4914-A9B9-98719E8B0E58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE5C8D1B-48F1-4AE5-BEB0-0B4DCF142D3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-60" yWindow="-60" windowWidth="28920" windowHeight="15720" xr2:uid="{9496D2BA-4ACD-41C0-814E-16707366DC5E}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="85">
   <si>
     <t>DAWN</t>
   </si>
@@ -252,9 +252,6 @@
     <t>-200℃</t>
   </si>
   <si>
-    <t>0℃/s / ?℃/s</t>
-  </si>
-  <si>
     <t xml:space="preserve">  ?℃/s</t>
   </si>
   <si>
@@ -264,10 +261,34 @@
     <t>?℃</t>
   </si>
   <si>
-    <t>0℃/m / ?℃/m</t>
-  </si>
-  <si>
     <t xml:space="preserve">  ?℃/m</t>
+  </si>
+  <si>
+    <t>20℃/-15℃</t>
+  </si>
+  <si>
+    <t>27℃/-8℃</t>
+  </si>
+  <si>
+    <t>4℃/-23℃</t>
+  </si>
+  <si>
+    <t>0℃/m / -2,6℃/m</t>
+  </si>
+  <si>
+    <t>0℃/m / -1,2℃/m</t>
+  </si>
+  <si>
+    <t>0℃/m / -3,7℃/m</t>
+  </si>
+  <si>
+    <t>0℃/s / -0,043℃/s</t>
+  </si>
+  <si>
+    <t>0℃/s / -0,02℃/s</t>
+  </si>
+  <si>
+    <t>0℃/s / -0,0616℃/s</t>
   </si>
 </sst>
 </file>
@@ -722,16 +743,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0C3F330-1E39-43F9-9FE4-6E0C18023283}">
   <dimension ref="A1:L22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="13.28515625" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" customWidth="1"/>
-    <col min="4" max="4" width="13" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" customWidth="1"/>
+    <col min="2" max="2" width="16" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" customWidth="1"/>
+    <col min="4" max="4" width="17.5703125" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" customWidth="1"/>
     <col min="6" max="6" width="3.42578125" customWidth="1"/>
     <col min="7" max="7" width="12" customWidth="1"/>
     <col min="8" max="8" width="12.28515625" customWidth="1"/>
@@ -909,21 +930,21 @@
       </c>
       <c r="L5" s="6"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>72</v>
+        <v>83</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>72</v>
+        <v>84</v>
       </c>
       <c r="F6" s="6"/>
       <c r="G6" s="3" t="s">
@@ -964,16 +985,16 @@
         <v>8</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I7" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J7" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K7" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="L7" s="6"/>
     </row>
@@ -982,32 +1003,32 @@
         <v>10</v>
       </c>
       <c r="B8" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>74</v>
-      </c>
       <c r="D8" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F8" s="6"/>
       <c r="G8" s="2" t="s">
         <v>10</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="L8" s="6"/>
     </row>
@@ -1268,32 +1289,32 @@
         <v>9</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="F17" s="6"/>
       <c r="G17" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H17" s="8" t="s">
-        <v>17</v>
+        <v>76</v>
       </c>
       <c r="I17" s="8" t="s">
-        <v>17</v>
+        <v>77</v>
       </c>
       <c r="J17" s="8" t="s">
-        <v>17</v>
+        <v>76</v>
       </c>
       <c r="K17" s="8" t="s">
-        <v>17</v>
+        <v>78</v>
       </c>
       <c r="L17" s="6"/>
     </row>
@@ -1336,16 +1357,16 @@
         <v>10</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F19" s="6"/>
       <c r="G19" s="1" t="s">

</xml_diff>

<commit_message>
[NTM:SPACE] Ike + Laythe temperature rebalance
</commit_message>
<xml_diff>
--- a/DEBUG_SHEET/TEMPS.xlsx
+++ b/DEBUG_SHEET/TEMPS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE5C8D1B-48F1-4AE5-BEB0-0B4DCF142D3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0758207D-83DC-4C81-B6F8-FF7A91ED188C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-60" yWindow="-60" windowWidth="28920" windowHeight="15720" xr2:uid="{9496D2BA-4ACD-41C0-814E-16707366DC5E}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="92">
   <si>
     <t>DAWN</t>
   </si>
@@ -174,18 +174,9 @@
     <t>0,262℃/s</t>
   </si>
   <si>
-    <t>0℃</t>
-  </si>
-  <si>
-    <t>30℃</t>
-  </si>
-  <si>
     <t>25℃</t>
   </si>
   <si>
-    <t>-10℃</t>
-  </si>
-  <si>
     <t>20℃</t>
   </si>
   <si>
@@ -195,9 +186,6 @@
     <t>18℃</t>
   </si>
   <si>
-    <t>7℃</t>
-  </si>
-  <si>
     <t>17℃</t>
   </si>
   <si>
@@ -270,9 +258,6 @@
     <t>27℃/-8℃</t>
   </si>
   <si>
-    <t>4℃/-23℃</t>
-  </si>
-  <si>
     <t>0℃/m / -2,6℃/m</t>
   </si>
   <si>
@@ -289,6 +274,42 @@
   </si>
   <si>
     <t>0℃/s / -0,0616℃/s</t>
+  </si>
+  <si>
+    <t>-4℃</t>
+  </si>
+  <si>
+    <t>-112℃</t>
+  </si>
+  <si>
+    <t>-58℃</t>
+  </si>
+  <si>
+    <t>-6℃</t>
+  </si>
+  <si>
+    <t>-7℃</t>
+  </si>
+  <si>
+    <t>13℃</t>
+  </si>
+  <si>
+    <t>24℃</t>
+  </si>
+  <si>
+    <t>35℃</t>
+  </si>
+  <si>
+    <t>32℃</t>
+  </si>
+  <si>
+    <t>12℃</t>
+  </si>
+  <si>
+    <t>7℃/-23℃</t>
+  </si>
+  <si>
+    <t>-14℃</t>
   </si>
 </sst>
 </file>
@@ -744,7 +765,7 @@
   <dimension ref="A1:L22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -867,16 +888,16 @@
         <v>6</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="F4" s="6"/>
       <c r="G4" s="1" t="s">
@@ -901,16 +922,16 @@
         <v>7</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="F5" s="6"/>
       <c r="G5" s="1" t="s">
@@ -935,32 +956,32 @@
         <v>9</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="F6" s="6"/>
       <c r="G6" s="3" t="s">
         <v>9</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="K6" s="5" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="L6" s="6"/>
     </row>
@@ -969,32 +990,32 @@
         <v>8</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="F7" s="6"/>
       <c r="G7" s="1" t="s">
         <v>8</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="I7" s="8" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="J7" s="8" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="K7" s="8" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="L7" s="6"/>
     </row>
@@ -1003,66 +1024,66 @@
         <v>10</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="F8" s="6"/>
       <c r="G8" s="2" t="s">
         <v>10</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="L8" s="6"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="F9" s="6"/>
       <c r="G9" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="H9" s="8" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="I9" s="8" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="J9" s="8" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="K9" s="8" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="L9" s="6"/>
     </row>
@@ -1071,32 +1092,32 @@
         <v>11</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="F10" s="6"/>
       <c r="G10" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H10" s="8" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="I10" s="8" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="J10" s="8" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="K10" s="8" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="L10" s="6"/>
     </row>
@@ -1169,16 +1190,16 @@
         <v>4</v>
       </c>
       <c r="H13" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="I13" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="J13" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="I13" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="J13" s="8" t="s">
-        <v>48</v>
-      </c>
       <c r="K13" s="8" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="L13" s="6"/>
     </row>
@@ -1203,16 +1224,16 @@
         <v>5</v>
       </c>
       <c r="H14" s="8" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="I14" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="J14" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="J14" s="8" t="s">
-        <v>51</v>
-      </c>
       <c r="K14" s="8" t="s">
-        <v>53</v>
+        <v>89</v>
       </c>
       <c r="L14" s="6"/>
     </row>
@@ -1221,29 +1242,29 @@
         <v>6</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="F15" s="6"/>
       <c r="G15" s="1" t="s">
         <v>6</v>
       </c>
       <c r="H15" s="8" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="I15" s="8" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="J15" s="8" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="K15" s="8" t="s">
         <v>36</v>
@@ -1255,16 +1276,16 @@
         <v>7</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="F16" s="6"/>
       <c r="G16" s="1" t="s">
@@ -1274,13 +1295,13 @@
         <v>36</v>
       </c>
       <c r="I16" s="8" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="J16" s="8" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="K16" s="8" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="L16" s="6"/>
     </row>
@@ -1289,32 +1310,32 @@
         <v>9</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="F17" s="6"/>
       <c r="G17" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H17" s="8" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="I17" s="8" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="J17" s="8" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="K17" s="8" t="s">
-        <v>78</v>
+        <v>90</v>
       </c>
       <c r="L17" s="6"/>
     </row>
@@ -1323,32 +1344,32 @@
         <v>8</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="F18" s="6"/>
       <c r="G18" s="1" t="s">
         <v>8</v>
       </c>
       <c r="H18" s="8" t="s">
-        <v>17</v>
+        <v>83</v>
       </c>
       <c r="I18" s="8" t="s">
-        <v>17</v>
+        <v>85</v>
       </c>
       <c r="J18" s="8" t="s">
-        <v>17</v>
+        <v>84</v>
       </c>
       <c r="K18" s="8" t="s">
-        <v>17</v>
+        <v>91</v>
       </c>
       <c r="L18" s="6"/>
     </row>
@@ -1357,16 +1378,16 @@
         <v>10</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="F19" s="6"/>
       <c r="G19" s="1" t="s">
@@ -1388,35 +1409,35 @@
     </row>
     <row r="20" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="F20" s="6"/>
       <c r="G20" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="H20" s="8" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="I20" s="8" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="J20" s="8" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="K20" s="8" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="L20" s="6"/>
     </row>
@@ -1425,32 +1446,32 @@
         <v>11</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="F21" s="6"/>
       <c r="G21" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H21" s="8" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="I21" s="8" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="J21" s="8" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="K21" s="8" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="L21" s="6"/>
     </row>

</xml_diff>

<commit_message>
[NTM:SPACE] Dres temperature rebalance {FINAL}
</commit_message>
<xml_diff>
--- a/DEBUG_SHEET/TEMPS.xlsx
+++ b/DEBUG_SHEET/TEMPS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0758207D-83DC-4C81-B6F8-FF7A91ED188C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20B95E7B-4930-4C84-BFDE-34E107811A8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-60" yWindow="-60" windowWidth="28920" windowHeight="15720" xr2:uid="{9496D2BA-4ACD-41C0-814E-16707366DC5E}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="100">
   <si>
     <t>DAWN</t>
   </si>
@@ -63,9 +63,6 @@
     <t>Ike</t>
   </si>
   <si>
-    <t>Duna/I</t>
-  </si>
-  <si>
     <t>Dres</t>
   </si>
   <si>
@@ -87,9 +84,6 @@
     <t>-180℃</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>-190℃</t>
   </si>
   <si>
@@ -192,9 +186,6 @@
     <t>23℃</t>
   </si>
   <si>
-    <t>Laythe/I</t>
-  </si>
-  <si>
     <t>-49℃/-93℃</t>
   </si>
   <si>
@@ -240,18 +231,6 @@
     <t>-200℃</t>
   </si>
   <si>
-    <t xml:space="preserve">  ?℃/s</t>
-  </si>
-  <si>
-    <t>?℃/s</t>
-  </si>
-  <si>
-    <t>?℃</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  ?℃/m</t>
-  </si>
-  <si>
     <t>20℃/-15℃</t>
   </si>
   <si>
@@ -310,6 +289,51 @@
   </si>
   <si>
     <t>-14℃</t>
+  </si>
+  <si>
+    <t>-38℃</t>
+  </si>
+  <si>
+    <t>-106℃</t>
+  </si>
+  <si>
+    <t>-163℃</t>
+  </si>
+  <si>
+    <t>-31℃</t>
+  </si>
+  <si>
+    <t>-52℃</t>
+  </si>
+  <si>
+    <t>-17℃</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  -2,8℃/m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  -1℃/m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  -4℃/m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  -0,046℃/s</t>
+  </si>
+  <si>
+    <t>-0,046℃/s</t>
+  </si>
+  <si>
+    <t>-0,016℃/s</t>
+  </si>
+  <si>
+    <t>-0,066℃/s</t>
+  </si>
+  <si>
+    <t>Laythe/Polar</t>
+  </si>
+  <si>
+    <t>Duna/Polar</t>
   </si>
 </sst>
 </file>
@@ -765,17 +789,18 @@
   <dimension ref="A1:L22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="12.28515625" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
     <col min="3" max="3" width="16.140625" customWidth="1"/>
     <col min="4" max="4" width="17.5703125" customWidth="1"/>
     <col min="5" max="5" width="17.28515625" customWidth="1"/>
     <col min="6" max="6" width="3.42578125" customWidth="1"/>
-    <col min="7" max="7" width="12" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" customWidth="1"/>
     <col min="8" max="8" width="12.28515625" customWidth="1"/>
     <col min="9" max="10" width="15.28515625" customWidth="1"/>
     <col min="11" max="11" width="13.5703125" customWidth="1"/>
@@ -783,7 +808,7 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B1" s="7" t="s">
         <v>0</v>
@@ -799,7 +824,7 @@
       </c>
       <c r="F1" s="6"/>
       <c r="G1" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H1" s="7" t="s">
         <v>0</v>
@@ -820,32 +845,32 @@
         <v>4</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="E2" s="4" t="s">
         <v>39</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>41</v>
       </c>
       <c r="F2" s="6"/>
       <c r="G2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="H2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="K2" s="4" t="s">
         <v>16</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>18</v>
       </c>
       <c r="L2" s="6"/>
     </row>
@@ -854,32 +879,32 @@
         <v>5</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F3" s="6"/>
       <c r="G3" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="L3" s="6"/>
     </row>
@@ -888,32 +913,32 @@
         <v>6</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F4" s="6"/>
       <c r="G4" s="1" t="s">
         <v>6</v>
       </c>
       <c r="H4" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="I4" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="K4" s="8" t="s">
         <v>33</v>
-      </c>
-      <c r="I4" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="J4" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="K4" s="8" t="s">
-        <v>35</v>
       </c>
       <c r="L4" s="6"/>
     </row>
@@ -922,66 +947,66 @@
         <v>7</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F5" s="6"/>
       <c r="G5" s="1" t="s">
         <v>7</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="I5" s="8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="J5" s="8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="K5" s="8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="L5" s="6"/>
     </row>
     <row r="6" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>9</v>
+        <v>99</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="F6" s="6"/>
       <c r="G6" s="3" t="s">
-        <v>9</v>
+        <v>99</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="K6" s="5" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="L6" s="6"/>
     </row>
@@ -990,134 +1015,134 @@
         <v>8</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F7" s="6"/>
       <c r="G7" s="1" t="s">
         <v>8</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="I7" s="8" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="J7" s="8" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="K7" s="8" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="L7" s="6"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>68</v>
+        <v>94</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>69</v>
+        <v>96</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>69</v>
+        <v>95</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>69</v>
+        <v>97</v>
       </c>
       <c r="F8" s="6"/>
       <c r="G8" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>70</v>
+        <v>86</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>70</v>
+        <v>85</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>70</v>
+        <v>86</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>70</v>
+        <v>87</v>
       </c>
       <c r="L8" s="6"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>52</v>
+        <v>98</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F9" s="6"/>
       <c r="G9" s="1" t="s">
-        <v>52</v>
+        <v>98</v>
       </c>
       <c r="H9" s="8" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="I9" s="8" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="J9" s="8" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="K9" s="8" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="L9" s="6"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F10" s="6"/>
       <c r="G10" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H10" s="8" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="I10" s="8" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="J10" s="8" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="K10" s="8" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="L10" s="6"/>
     </row>
@@ -1137,7 +1162,7 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B12" s="7" t="s">
         <v>0</v>
@@ -1153,7 +1178,7 @@
       </c>
       <c r="F12" s="6"/>
       <c r="G12" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H12" s="7" t="s">
         <v>0</v>
@@ -1174,32 +1199,32 @@
         <v>4</v>
       </c>
       <c r="B13" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="D13" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="E13" s="4" t="s">
         <v>29</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>31</v>
       </c>
       <c r="F13" s="6"/>
       <c r="G13" s="1" t="s">
         <v>4</v>
       </c>
       <c r="H13" s="8" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="I13" s="8" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="J13" s="8" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="K13" s="8" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="L13" s="6"/>
     </row>
@@ -1208,32 +1233,32 @@
         <v>5</v>
       </c>
       <c r="B14" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="D14" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="E14" s="4" t="s">
         <v>30</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>32</v>
       </c>
       <c r="F14" s="6"/>
       <c r="G14" s="1" t="s">
         <v>5</v>
       </c>
       <c r="H14" s="8" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="I14" s="8" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="J14" s="8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="K14" s="8" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="L14" s="6"/>
     </row>
@@ -1242,32 +1267,32 @@
         <v>6</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="F15" s="6"/>
       <c r="G15" s="1" t="s">
         <v>6</v>
       </c>
       <c r="H15" s="8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I15" s="8" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="J15" s="8" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="K15" s="8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="L15" s="6"/>
     </row>
@@ -1276,66 +1301,66 @@
         <v>7</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="F16" s="6"/>
       <c r="G16" s="1" t="s">
         <v>7</v>
       </c>
       <c r="H16" s="8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="I16" s="8" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="J16" s="8" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="K16" s="8" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="L16" s="6"/>
     </row>
     <row r="17" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>9</v>
+        <v>99</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="F17" s="6"/>
       <c r="G17" s="1" t="s">
-        <v>9</v>
+        <v>99</v>
       </c>
       <c r="H17" s="8" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="I17" s="8" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="J17" s="8" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="K17" s="8" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="L17" s="6"/>
     </row>
@@ -1344,134 +1369,134 @@
         <v>8</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="F18" s="6"/>
       <c r="G18" s="1" t="s">
         <v>8</v>
       </c>
       <c r="H18" s="8" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="I18" s="8" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="J18" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="K18" s="8" t="s">
         <v>84</v>
-      </c>
-      <c r="K18" s="8" t="s">
-        <v>91</v>
       </c>
       <c r="L18" s="6"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>71</v>
+        <v>91</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>71</v>
+        <v>92</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>71</v>
+        <v>91</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>71</v>
+        <v>93</v>
       </c>
       <c r="F19" s="6"/>
       <c r="G19" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H19" s="8" t="s">
-        <v>17</v>
+        <v>88</v>
       </c>
       <c r="I19" s="8" t="s">
-        <v>17</v>
+        <v>90</v>
       </c>
       <c r="J19" s="8" t="s">
-        <v>17</v>
+        <v>88</v>
       </c>
       <c r="K19" s="8" t="s">
-        <v>17</v>
+        <v>89</v>
       </c>
       <c r="L19" s="6"/>
     </row>
     <row r="20" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>52</v>
+        <v>98</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="F20" s="6"/>
       <c r="G20" s="1" t="s">
-        <v>52</v>
+        <v>98</v>
       </c>
       <c r="H20" s="8" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="I20" s="8" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="J20" s="8" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="K20" s="8" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="L20" s="6"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="F21" s="6"/>
       <c r="G21" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H21" s="8" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="I21" s="8" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="J21" s="8" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="K21" s="8" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="L21" s="6"/>
     </row>

</xml_diff>